<commit_message>
Usar validación cruzada para generar el modelo con los mejores parametros
</commit_message>
<xml_diff>
--- a/predictions/Retionopatía Proliferativa_Pipeline.xlsx
+++ b/predictions/Retionopatía Proliferativa_Pipeline.xlsx
@@ -447,10 +447,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.2543120278050841</v>
+        <v>0.256802507014269</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9981558851202715</v>
+        <v>0.9981366696299599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>